<commit_message>
filter performance increase to 88.53 % for 3000 articles
</commit_message>
<xml_diff>
--- a/company_keyword.xlsx
+++ b/company_keyword.xlsx
@@ -148,9 +148,6 @@
     <t>OTHERS</t>
   </si>
   <si>
-    <t>Reliance Industries,Mukesh Ambani,Anil Ambani,Reliance Commercial Corporation,RELIANCE,RIL</t>
-  </si>
-  <si>
     <t>AIRTL</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Tata Motors Limited,TELCO,TATAMOTORS,Tata Group,Tata Motors Cars,Guenter Butschek,Chandrasekaran</t>
+  </si>
+  <si>
+    <t>Reliance Industries,Mukesh Ambani,Anil Ambani,Reliance Commercial Corporation,RELIANCE,RIL,Jio</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -676,7 +676,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
@@ -764,87 +764,87 @@
         <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>